<commit_message>
Last commit for PAIN
</commit_message>
<xml_diff>
--- a/data-original/ADVANCE-cd4-all.xlsx
+++ b/data-original/ADVANCE-cd4-all.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/Dropbox/_home/data-analysis-other/toni-wadley/advance-pain/data-original/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/Dropbox/_home/data-analysis-other/toni-wadley/ADVANCE-pain-variability/data-original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012434A-A37D-7144-B361-F9E1A20392CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D796D97E-69C8-8C4C-A939-EEB2C4DFA1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{77695A67-52C9-47C7-934D-0AA051AB09BA}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="32440" windowHeight="20540" activeTab="1" xr2:uid="{77695A67-52C9-47C7-934D-0AA051AB09BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="code sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$3574</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21453" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21469" uniqueCount="1090">
   <si>
     <t>ranid</t>
   </si>
@@ -3280,6 +3281,30 @@
   </si>
   <si>
     <t>03-0023</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>Treatment group</t>
+  </si>
+  <si>
+    <t>Age in years</t>
+  </si>
+  <si>
+    <t>Sex (M = male, F = female)</t>
+  </si>
+  <si>
+    <t>Name of blood test</t>
+  </si>
+  <si>
+    <t>Numeric value of test result (cells count)</t>
+  </si>
+  <si>
+    <t>Units of measure (cell count per microlitre)</t>
+  </si>
+  <si>
+    <t>Visit number (W = week)</t>
   </si>
 </sst>
 </file>
@@ -3642,9 +3667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3262F0-AEC0-41A0-A2E8-09BBDDBE7BFD}">
   <dimension ref="A1:H3574"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -96582,4 +96607,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F3C488-3358-224A-933B-79E71EE020E2}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>